<commit_message>
Redesing of the HTM with movement based on gravity model.
</commit_message>
<xml_diff>
--- a/HTM/HalibutData.xlsx
+++ b/HTM/HalibutData.xlsx
@@ -117,7 +117,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -137,16 +137,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +167,11 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -165,6 +181,11 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2764,10 +2785,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2805,28 +2826,28 @@
       <c r="A2">
         <v>1977</v>
       </c>
-      <c r="B2">
-        <v>-999</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C2" s="4">
         <v>13.7</v>
       </c>
-      <c r="D2">
-        <v>-999</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E2" s="4">
         <v>58.4</v>
       </c>
-      <c r="F2">
-        <v>-999</v>
-      </c>
-      <c r="G2">
-        <v>-999</v>
-      </c>
-      <c r="H2">
-        <v>-999</v>
-      </c>
-      <c r="I2">
+      <c r="F2" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H2" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I2" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -2834,28 +2855,28 @@
       <c r="A3">
         <v>1978</v>
       </c>
-      <c r="B3">
-        <v>-999</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C3" s="4">
         <v>19.100000000000001</v>
       </c>
-      <c r="D3">
-        <v>-999</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E3" s="4">
         <v>26.9</v>
       </c>
-      <c r="F3">
-        <v>-999</v>
-      </c>
-      <c r="G3">
-        <v>-999</v>
-      </c>
-      <c r="H3">
-        <v>-999</v>
-      </c>
-      <c r="I3">
+      <c r="F3" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I3" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -2863,28 +2884,28 @@
       <c r="A4">
         <v>1979</v>
       </c>
-      <c r="B4">
-        <v>-999</v>
-      </c>
-      <c r="C4">
-        <v>-999</v>
-      </c>
-      <c r="D4">
-        <v>-999</v>
-      </c>
-      <c r="E4">
+      <c r="B4" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>-999</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E4" s="4">
         <v>41</v>
       </c>
-      <c r="F4">
-        <v>-999</v>
-      </c>
-      <c r="G4">
-        <v>-999</v>
-      </c>
-      <c r="H4">
-        <v>-999</v>
-      </c>
-      <c r="I4">
+      <c r="F4" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I4" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -2892,28 +2913,28 @@
       <c r="A5">
         <v>1980</v>
       </c>
-      <c r="B5">
-        <v>-999</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C5" s="4">
         <v>25.5</v>
       </c>
-      <c r="D5">
-        <v>-999</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E5" s="4">
         <v>76.2</v>
       </c>
-      <c r="F5">
-        <v>-999</v>
-      </c>
-      <c r="G5">
-        <v>-999</v>
-      </c>
-      <c r="H5">
-        <v>-999</v>
-      </c>
-      <c r="I5">
+      <c r="F5" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I5" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -2921,28 +2942,28 @@
       <c r="A6">
         <v>1981</v>
       </c>
-      <c r="B6">
-        <v>-999</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C6" s="4">
         <v>16.5</v>
       </c>
-      <c r="D6">
-        <v>-999</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E6" s="4">
         <v>131.4</v>
       </c>
-      <c r="F6">
-        <v>-999</v>
-      </c>
-      <c r="G6">
-        <v>-999</v>
-      </c>
-      <c r="H6">
-        <v>-999</v>
-      </c>
-      <c r="I6">
+      <c r="F6" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I6" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -2950,28 +2971,28 @@
       <c r="A7">
         <v>1982</v>
       </c>
-      <c r="B7">
-        <v>-999</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C7" s="4">
         <v>20.6</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>113.7</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>130.30000000000001</v>
       </c>
-      <c r="F7">
-        <v>-999</v>
-      </c>
-      <c r="G7">
-        <v>-999</v>
-      </c>
-      <c r="H7">
-        <v>-999</v>
-      </c>
-      <c r="I7">
+      <c r="F7" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I7" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -2979,28 +3000,28 @@
       <c r="A8">
         <v>1983</v>
       </c>
-      <c r="B8">
-        <v>-999</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C8" s="4">
         <v>18</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>142.19999999999999</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>119</v>
       </c>
-      <c r="F8">
-        <v>-999</v>
-      </c>
-      <c r="G8">
-        <v>-999</v>
-      </c>
-      <c r="H8">
-        <v>-999</v>
-      </c>
-      <c r="I8">
+      <c r="F8" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I8" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -3008,28 +3029,28 @@
       <c r="A9">
         <v>1984</v>
       </c>
-      <c r="B9">
-        <v>-999</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C9" s="4">
         <v>57.4</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>259.60000000000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>361.2</v>
       </c>
-      <c r="F9">
-        <v>-999</v>
-      </c>
-      <c r="G9">
-        <v>-999</v>
-      </c>
-      <c r="H9">
-        <v>-999</v>
-      </c>
-      <c r="I9">
+      <c r="F9" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G9" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H9" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I9" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -3037,28 +3058,28 @@
       <c r="A10">
         <v>1985</v>
       </c>
-      <c r="B10">
-        <v>-999</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C10" s="4">
         <v>41.7</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>260.5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>377.5</v>
       </c>
-      <c r="F10">
-        <v>-999</v>
-      </c>
-      <c r="G10">
-        <v>-999</v>
-      </c>
-      <c r="H10">
-        <v>-999</v>
-      </c>
-      <c r="I10">
+      <c r="F10" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I10" s="4">
         <v>-999</v>
       </c>
     </row>
@@ -3066,782 +3087,608 @@
       <c r="A11">
         <v>1986</v>
       </c>
-      <c r="B11">
-        <v>-999</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C11" s="4">
         <v>37.799999999999997</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>282.60000000000002</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>305.10000000000002</v>
       </c>
-      <c r="F11">
-        <v>-999</v>
-      </c>
-      <c r="G11">
-        <v>-999</v>
-      </c>
-      <c r="H11">
-        <v>-999</v>
-      </c>
-      <c r="I11">
+      <c r="F11" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G11" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I11" s="4">
         <v>-999</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>1987</v>
-      </c>
-      <c r="B12">
-        <v>-999</v>
-      </c>
-      <c r="C12">
-        <v>-999</v>
-      </c>
-      <c r="D12">
-        <v>-999</v>
-      </c>
-      <c r="E12">
-        <v>-999</v>
-      </c>
-      <c r="F12">
-        <v>-999</v>
-      </c>
-      <c r="G12">
-        <v>-999</v>
-      </c>
-      <c r="H12">
-        <v>-999</v>
-      </c>
-      <c r="I12">
+        <v>1993</v>
+      </c>
+      <c r="B12" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C12" s="4">
+        <v>95.7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E12" s="4">
+        <v>261.10000000000002</v>
+      </c>
+      <c r="F12" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H12" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I12" s="4">
         <v>-999</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>1988</v>
-      </c>
-      <c r="B13">
-        <v>-999</v>
-      </c>
-      <c r="C13">
-        <v>-999</v>
-      </c>
-      <c r="D13">
-        <v>-999</v>
-      </c>
-      <c r="E13">
-        <v>-999</v>
-      </c>
-      <c r="F13">
-        <v>-999</v>
-      </c>
-      <c r="G13">
-        <v>-999</v>
-      </c>
-      <c r="H13">
-        <v>-999</v>
-      </c>
-      <c r="I13">
+        <v>1994</v>
+      </c>
+      <c r="B13" s="4">
+        <v>-999</v>
+      </c>
+      <c r="C13" s="4">
+        <v>-999</v>
+      </c>
+      <c r="D13" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E13" s="4">
+        <v>253.9</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G13" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I13" s="4">
         <v>-999</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
-        <v>1989</v>
-      </c>
-      <c r="B14">
-        <v>-999</v>
-      </c>
-      <c r="C14">
-        <v>-999</v>
-      </c>
-      <c r="D14">
-        <v>-999</v>
-      </c>
-      <c r="E14">
-        <v>-999</v>
-      </c>
-      <c r="F14">
-        <v>-999</v>
-      </c>
-      <c r="G14">
-        <v>-999</v>
-      </c>
-      <c r="H14">
-        <v>-999</v>
-      </c>
-      <c r="I14">
+        <v>1995</v>
+      </c>
+      <c r="B14" s="4">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4">
+        <v>159.1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>-999</v>
+      </c>
+      <c r="E14" s="4">
+        <v>300.10000000000002</v>
+      </c>
+      <c r="F14" s="4">
+        <v>-999</v>
+      </c>
+      <c r="G14" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I14" s="4">
         <v>-999</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>1990</v>
-      </c>
-      <c r="B15">
-        <v>-999</v>
-      </c>
-      <c r="C15">
-        <v>-999</v>
-      </c>
-      <c r="D15">
-        <v>-999</v>
-      </c>
-      <c r="E15">
-        <v>-999</v>
-      </c>
-      <c r="F15">
-        <v>-999</v>
-      </c>
-      <c r="G15">
-        <v>-999</v>
-      </c>
-      <c r="H15">
-        <v>-999</v>
-      </c>
-      <c r="I15">
+        <v>1996</v>
+      </c>
+      <c r="B15" s="4">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="C15" s="4">
+        <v>165.9</v>
+      </c>
+      <c r="D15" s="4">
+        <v>306.2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>317.3</v>
+      </c>
+      <c r="F15" s="4">
+        <v>352.2</v>
+      </c>
+      <c r="G15" s="4">
+        <v>-999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-999</v>
+      </c>
+      <c r="I15" s="4">
         <v>-999</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>1991</v>
-      </c>
-      <c r="B16">
-        <v>-999</v>
-      </c>
-      <c r="C16">
-        <v>-999</v>
-      </c>
-      <c r="D16">
-        <v>-999</v>
-      </c>
-      <c r="E16">
-        <v>-999</v>
-      </c>
-      <c r="F16">
-        <v>-999</v>
-      </c>
-      <c r="G16">
-        <v>-999</v>
-      </c>
-      <c r="H16">
-        <v>-999</v>
-      </c>
-      <c r="I16">
-        <v>-999</v>
+        <v>1997</v>
+      </c>
+      <c r="B16" s="4">
+        <v>36.4</v>
+      </c>
+      <c r="C16" s="4">
+        <v>144.1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>410.6</v>
+      </c>
+      <c r="E16" s="4">
+        <v>330.6</v>
+      </c>
+      <c r="F16" s="4">
+        <v>413.9</v>
+      </c>
+      <c r="G16" s="4">
+        <v>245.4</v>
+      </c>
+      <c r="H16" s="4">
+        <v>281.60000000000002</v>
+      </c>
+      <c r="I16" s="4">
+        <v>23.2</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>1992</v>
-      </c>
-      <c r="B17">
-        <v>-999</v>
-      </c>
-      <c r="C17">
-        <v>-999</v>
-      </c>
-      <c r="D17">
-        <v>-999</v>
-      </c>
-      <c r="E17">
-        <v>-999</v>
-      </c>
-      <c r="F17">
-        <v>-999</v>
-      </c>
-      <c r="G17">
-        <v>-999</v>
-      </c>
-      <c r="H17">
-        <v>-999</v>
-      </c>
-      <c r="I17">
-        <v>-999</v>
+        <v>1998</v>
+      </c>
+      <c r="B17" s="4">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="C17" s="4">
+        <v>83.3</v>
+      </c>
+      <c r="D17" s="4">
+        <v>234.8</v>
+      </c>
+      <c r="E17" s="4">
+        <v>281.2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>434.9</v>
+      </c>
+      <c r="G17" s="4">
+        <v>299</v>
+      </c>
+      <c r="H17" s="4">
+        <v>215.6</v>
+      </c>
+      <c r="I17" s="4">
+        <v>44.5</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>1993</v>
-      </c>
-      <c r="B18">
-        <v>-999</v>
-      </c>
-      <c r="C18">
-        <v>95.7</v>
-      </c>
-      <c r="D18">
-        <v>-999</v>
-      </c>
-      <c r="E18">
-        <v>261.10000000000002</v>
-      </c>
-      <c r="F18">
-        <v>-999</v>
-      </c>
-      <c r="G18">
-        <v>-999</v>
-      </c>
-      <c r="H18">
-        <v>-999</v>
-      </c>
-      <c r="I18">
-        <v>-999</v>
+        <v>1999</v>
+      </c>
+      <c r="B18" s="4">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="C18" s="4">
+        <v>88.1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>208.9</v>
+      </c>
+      <c r="E18" s="4">
+        <v>240.7</v>
+      </c>
+      <c r="F18" s="4">
+        <v>437.9</v>
+      </c>
+      <c r="G18" s="4">
+        <v>290.3</v>
+      </c>
+      <c r="H18" s="4">
+        <v>203.1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>42.1</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19">
-        <v>1994</v>
-      </c>
-      <c r="B19">
-        <v>-999</v>
-      </c>
-      <c r="C19">
-        <v>-999</v>
-      </c>
-      <c r="D19">
-        <v>-999</v>
-      </c>
-      <c r="E19">
-        <v>253.9</v>
-      </c>
-      <c r="F19">
-        <v>-999</v>
-      </c>
-      <c r="G19">
-        <v>-999</v>
-      </c>
-      <c r="H19">
-        <v>-999</v>
-      </c>
-      <c r="I19">
-        <v>-999</v>
+        <v>2000</v>
+      </c>
+      <c r="B19" s="4">
+        <v>40.6</v>
+      </c>
+      <c r="C19" s="4">
+        <v>91.2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>240.1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>271.7</v>
+      </c>
+      <c r="F19" s="4">
+        <v>373.1</v>
+      </c>
+      <c r="G19" s="4">
+        <v>275.8</v>
+      </c>
+      <c r="H19" s="4">
+        <v>216.3</v>
+      </c>
+      <c r="I19" s="4">
+        <v>31.5</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20">
-        <v>1995</v>
-      </c>
-      <c r="B20">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>159.1</v>
-      </c>
-      <c r="D20">
-        <v>-999</v>
-      </c>
-      <c r="E20">
-        <v>300.10000000000002</v>
-      </c>
-      <c r="F20">
-        <v>-999</v>
-      </c>
-      <c r="G20">
-        <v>-999</v>
-      </c>
-      <c r="H20">
-        <v>-999</v>
-      </c>
-      <c r="I20">
-        <v>-999</v>
+        <v>2001</v>
+      </c>
+      <c r="B20" s="4">
+        <v>43</v>
+      </c>
+      <c r="C20" s="4">
+        <v>101.1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>244.1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>256.10000000000002</v>
+      </c>
+      <c r="F20" s="4">
+        <v>357.1</v>
+      </c>
+      <c r="G20" s="4">
+        <v>198.8</v>
+      </c>
+      <c r="H20" s="4">
+        <v>171.3</v>
+      </c>
+      <c r="I20" s="4">
+        <v>31.3</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21">
-        <v>1996</v>
-      </c>
-      <c r="B21">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="C21">
-        <v>165.9</v>
-      </c>
-      <c r="D21">
-        <v>306.2</v>
-      </c>
-      <c r="E21">
-        <v>317.3</v>
-      </c>
-      <c r="F21">
-        <v>352.2</v>
-      </c>
-      <c r="G21">
-        <v>-999</v>
-      </c>
-      <c r="H21">
-        <v>-999</v>
-      </c>
-      <c r="I21">
-        <v>-999</v>
+        <v>2002</v>
+      </c>
+      <c r="B21" s="4">
+        <v>34.5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>91.8</v>
+      </c>
+      <c r="D21" s="4">
+        <v>267.8</v>
+      </c>
+      <c r="E21" s="4">
+        <v>299.39999999999998</v>
+      </c>
+      <c r="F21" s="4">
+        <v>297.2</v>
+      </c>
+      <c r="G21" s="4">
+        <v>168.4</v>
+      </c>
+      <c r="H21" s="4">
+        <v>119.1</v>
+      </c>
+      <c r="I21" s="4">
+        <v>31.1</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22">
-        <v>1997</v>
-      </c>
-      <c r="B22">
-        <v>36.4</v>
-      </c>
-      <c r="C22">
-        <v>144.1</v>
-      </c>
-      <c r="D22">
-        <v>410.6</v>
-      </c>
-      <c r="E22">
-        <v>330.6</v>
-      </c>
-      <c r="F22">
-        <v>413.9</v>
-      </c>
-      <c r="G22">
-        <v>245.4</v>
-      </c>
-      <c r="H22">
-        <v>281.60000000000002</v>
-      </c>
-      <c r="I22">
-        <v>23.2</v>
+        <v>2003</v>
+      </c>
+      <c r="B22" s="4">
+        <v>22.8</v>
+      </c>
+      <c r="C22" s="4">
+        <v>72.7</v>
+      </c>
+      <c r="D22" s="4">
+        <v>228.3</v>
+      </c>
+      <c r="E22" s="4">
+        <v>229.3</v>
+      </c>
+      <c r="F22" s="4">
+        <v>261.60000000000002</v>
+      </c>
+      <c r="G22" s="4">
+        <v>154.1</v>
+      </c>
+      <c r="H22" s="4">
+        <v>104.1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23">
-        <v>1998</v>
-      </c>
-      <c r="B23">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="C23">
-        <v>83.3</v>
-      </c>
-      <c r="D23">
-        <v>234.8</v>
-      </c>
-      <c r="E23">
-        <v>281.2</v>
-      </c>
-      <c r="F23">
-        <v>434.9</v>
-      </c>
-      <c r="G23">
-        <v>299</v>
-      </c>
-      <c r="H23">
-        <v>215.6</v>
-      </c>
-      <c r="I23">
-        <v>44.5</v>
+        <v>2004</v>
+      </c>
+      <c r="B23" s="4">
+        <v>27.9</v>
+      </c>
+      <c r="C23" s="4">
+        <v>85.8</v>
+      </c>
+      <c r="D23" s="4">
+        <v>176</v>
+      </c>
+      <c r="E23" s="4">
+        <v>269.7</v>
+      </c>
+      <c r="F23" s="4">
+        <v>236.3</v>
+      </c>
+      <c r="G23" s="4">
+        <v>137.4</v>
+      </c>
+      <c r="H23" s="4">
+        <v>73.3</v>
+      </c>
+      <c r="I23" s="4">
+        <v>23.3</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24">
-        <v>1999</v>
-      </c>
-      <c r="B24">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="C24">
-        <v>88.1</v>
-      </c>
-      <c r="D24">
-        <v>208.9</v>
-      </c>
-      <c r="E24">
-        <v>240.7</v>
-      </c>
-      <c r="F24">
-        <v>437.9</v>
-      </c>
-      <c r="G24">
-        <v>290.3</v>
-      </c>
-      <c r="H24">
-        <v>203.1</v>
-      </c>
-      <c r="I24">
-        <v>42.1</v>
+        <v>2005</v>
+      </c>
+      <c r="B24" s="4">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D24" s="4">
+        <v>174.7</v>
+      </c>
+      <c r="E24" s="4">
+        <v>275.89999999999998</v>
+      </c>
+      <c r="F24" s="4">
+        <v>211.2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>106.8</v>
+      </c>
+      <c r="H24" s="4">
+        <v>86.2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25">
-        <v>2000</v>
-      </c>
-      <c r="B25">
-        <v>40.6</v>
-      </c>
-      <c r="C25">
-        <v>91.2</v>
-      </c>
-      <c r="D25">
-        <v>240.1</v>
-      </c>
-      <c r="E25">
-        <v>271.7</v>
-      </c>
-      <c r="F25">
-        <v>373.1</v>
-      </c>
-      <c r="G25">
-        <v>275.8</v>
-      </c>
-      <c r="H25">
-        <v>216.3</v>
-      </c>
-      <c r="I25">
-        <v>31.5</v>
+        <v>2006</v>
+      </c>
+      <c r="B25" s="4">
+        <v>16.8</v>
+      </c>
+      <c r="C25" s="4">
+        <v>58.7</v>
+      </c>
+      <c r="D25" s="4">
+        <v>146.69999999999999</v>
+      </c>
+      <c r="E25" s="4">
+        <v>232.5</v>
+      </c>
+      <c r="F25" s="4">
+        <v>181.2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>84.9</v>
+      </c>
+      <c r="H25" s="4">
+        <v>95.5</v>
+      </c>
+      <c r="I25" s="4">
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26">
-        <v>2001</v>
-      </c>
-      <c r="B26">
-        <v>43</v>
-      </c>
-      <c r="C26">
-        <v>101.1</v>
-      </c>
-      <c r="D26">
-        <v>244.1</v>
-      </c>
-      <c r="E26">
-        <v>256.10000000000002</v>
-      </c>
-      <c r="F26">
-        <v>357.1</v>
-      </c>
-      <c r="G26">
-        <v>198.8</v>
-      </c>
-      <c r="H26">
-        <v>171.3</v>
-      </c>
-      <c r="I26">
-        <v>31.3</v>
+        <v>2007</v>
+      </c>
+      <c r="B26" s="4">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C26" s="4">
+        <v>57.2</v>
+      </c>
+      <c r="D26" s="4">
+        <v>142.6</v>
+      </c>
+      <c r="E26" s="4">
+        <v>211.6</v>
+      </c>
+      <c r="F26" s="4">
+        <v>191.3</v>
+      </c>
+      <c r="G26" s="4">
+        <v>66.5</v>
+      </c>
+      <c r="H26" s="4">
+        <v>87.2</v>
+      </c>
+      <c r="I26" s="4">
+        <v>13.3</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>2002</v>
-      </c>
-      <c r="B27">
-        <v>34.5</v>
-      </c>
-      <c r="C27">
-        <v>91.8</v>
-      </c>
-      <c r="D27">
-        <v>267.8</v>
-      </c>
-      <c r="E27">
-        <v>299.39999999999998</v>
-      </c>
-      <c r="F27">
-        <v>297.2</v>
-      </c>
-      <c r="G27">
-        <v>168.4</v>
-      </c>
-      <c r="H27">
-        <v>119.1</v>
-      </c>
-      <c r="I27">
-        <v>31.1</v>
+        <v>2008</v>
+      </c>
+      <c r="B27" s="4">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C27" s="4">
+        <v>89.8</v>
+      </c>
+      <c r="D27" s="4">
+        <v>106.4</v>
+      </c>
+      <c r="E27" s="4">
+        <v>189.1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>126</v>
+      </c>
+      <c r="G27" s="4">
+        <v>84.1</v>
+      </c>
+      <c r="H27" s="4">
+        <v>103.3</v>
+      </c>
+      <c r="I27" s="4">
+        <v>12.1</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
-        <v>2003</v>
-      </c>
-      <c r="B28">
-        <v>22.8</v>
-      </c>
-      <c r="C28">
-        <v>72.7</v>
-      </c>
-      <c r="D28">
-        <v>228.3</v>
-      </c>
-      <c r="E28">
-        <v>229.3</v>
-      </c>
-      <c r="F28">
-        <v>261.60000000000002</v>
-      </c>
-      <c r="G28">
-        <v>154.1</v>
-      </c>
-      <c r="H28">
-        <v>104.1</v>
-      </c>
-      <c r="I28">
-        <v>29</v>
+        <v>2009</v>
+      </c>
+      <c r="B28" s="4">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C28" s="4">
+        <v>86.3</v>
+      </c>
+      <c r="D28" s="4">
+        <v>115.6</v>
+      </c>
+      <c r="E28" s="4">
+        <v>148.80000000000001</v>
+      </c>
+      <c r="F28" s="4">
+        <v>113</v>
+      </c>
+      <c r="G28" s="4">
+        <v>84.1</v>
+      </c>
+      <c r="H28" s="4">
+        <v>106.8</v>
+      </c>
+      <c r="I28" s="4">
+        <v>14.5</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>2004</v>
-      </c>
-      <c r="B29">
-        <v>27.9</v>
-      </c>
-      <c r="C29">
-        <v>85.8</v>
-      </c>
-      <c r="D29">
-        <v>176</v>
-      </c>
-      <c r="E29">
-        <v>269.7</v>
-      </c>
-      <c r="F29">
-        <v>236.3</v>
-      </c>
-      <c r="G29">
-        <v>137.4</v>
-      </c>
-      <c r="H29">
-        <v>73.3</v>
-      </c>
-      <c r="I29">
-        <v>23.3</v>
+        <v>2010</v>
+      </c>
+      <c r="B29" s="4">
+        <v>17.3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>88.8</v>
+      </c>
+      <c r="D29" s="4">
+        <v>110.3</v>
+      </c>
+      <c r="E29" s="4">
+        <v>117.1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>91.4</v>
+      </c>
+      <c r="G29" s="4">
+        <v>73</v>
+      </c>
+      <c r="H29" s="4">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="I29" s="4">
+        <v>13.1</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>2005</v>
-      </c>
-      <c r="B30">
-        <v>29</v>
-      </c>
-      <c r="C30">
-        <v>71.900000000000006</v>
-      </c>
-      <c r="D30">
-        <v>174.7</v>
-      </c>
-      <c r="E30">
-        <v>275.89999999999998</v>
-      </c>
-      <c r="F30">
-        <v>211.2</v>
-      </c>
-      <c r="G30">
-        <v>106.8</v>
-      </c>
-      <c r="H30">
-        <v>86.2</v>
-      </c>
-      <c r="I30">
-        <v>17.399999999999999</v>
+        <v>2011</v>
+      </c>
+      <c r="B30" s="4">
+        <v>27</v>
+      </c>
+      <c r="C30" s="4">
+        <v>79.8</v>
+      </c>
+      <c r="D30" s="4">
+        <v>136.30000000000001</v>
+      </c>
+      <c r="E30" s="4">
+        <v>120.5</v>
+      </c>
+      <c r="F30" s="4">
+        <v>79.8</v>
+      </c>
+      <c r="G30" s="4">
+        <v>58.4</v>
+      </c>
+      <c r="H30" s="4">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="I30" s="4">
+        <v>10.1</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>2006</v>
-      </c>
-      <c r="B31">
-        <v>16.8</v>
-      </c>
-      <c r="C31">
-        <v>58.7</v>
-      </c>
-      <c r="D31">
-        <v>146.69999999999999</v>
-      </c>
-      <c r="E31">
-        <v>232.5</v>
-      </c>
-      <c r="F31">
-        <v>181.2</v>
-      </c>
-      <c r="G31">
-        <v>84.9</v>
-      </c>
-      <c r="H31">
-        <v>95.5</v>
-      </c>
-      <c r="I31">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32">
-        <v>2007</v>
-      </c>
-      <c r="B32">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="C32">
-        <v>57.2</v>
-      </c>
-      <c r="D32">
-        <v>142.6</v>
-      </c>
-      <c r="E32">
-        <v>211.6</v>
-      </c>
-      <c r="F32">
-        <v>191.3</v>
-      </c>
-      <c r="G32">
-        <v>66.5</v>
-      </c>
-      <c r="H32">
-        <v>87.2</v>
-      </c>
-      <c r="I32">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33">
-        <v>2008</v>
-      </c>
-      <c r="B33">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="C33">
-        <v>89.8</v>
-      </c>
-      <c r="D33">
-        <v>106.4</v>
-      </c>
-      <c r="E33">
-        <v>189.1</v>
-      </c>
-      <c r="F33">
-        <v>126</v>
-      </c>
-      <c r="G33">
-        <v>84.1</v>
-      </c>
-      <c r="H33">
-        <v>103.3</v>
-      </c>
-      <c r="I33">
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34">
-        <v>2009</v>
-      </c>
-      <c r="B34">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C34">
-        <v>86.3</v>
-      </c>
-      <c r="D34">
-        <v>115.6</v>
-      </c>
-      <c r="E34">
-        <v>148.80000000000001</v>
-      </c>
-      <c r="F34">
-        <v>113</v>
-      </c>
-      <c r="G34">
-        <v>84.1</v>
-      </c>
-      <c r="H34">
-        <v>106.8</v>
-      </c>
-      <c r="I34">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35">
-        <v>2010</v>
-      </c>
-      <c r="B35">
-        <v>17.3</v>
-      </c>
-      <c r="C35">
-        <v>88.8</v>
-      </c>
-      <c r="D35">
-        <v>110.3</v>
-      </c>
-      <c r="E35">
-        <v>117.1</v>
-      </c>
-      <c r="F35">
-        <v>91.4</v>
-      </c>
-      <c r="G35">
-        <v>73</v>
-      </c>
-      <c r="H35">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="I35">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36">
-        <v>2011</v>
-      </c>
-      <c r="B36">
-        <v>27</v>
-      </c>
-      <c r="C36">
-        <v>79.8</v>
-      </c>
-      <c r="D36">
-        <v>136.30000000000001</v>
-      </c>
-      <c r="E36">
-        <v>120.5</v>
-      </c>
-      <c r="F36">
-        <v>79.8</v>
-      </c>
-      <c r="G36">
-        <v>58.4</v>
-      </c>
-      <c r="H36">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="I36">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37">
         <v>2012</v>
       </c>
-      <c r="B37">
+      <c r="B31" s="4">
         <v>28.5</v>
       </c>
-      <c r="C37">
+      <c r="C31" s="4">
         <v>103.4</v>
       </c>
-      <c r="D37">
+      <c r="D31" s="4">
         <v>161.4</v>
       </c>
-      <c r="E37">
+      <c r="E31" s="4">
         <v>137</v>
       </c>
-      <c r="F37">
+      <c r="F31" s="4">
         <v>86.8</v>
       </c>
-      <c r="G37">
+      <c r="G31" s="4">
         <v>63.6</v>
       </c>
-      <c r="H37">
+      <c r="H31" s="4">
         <v>48.3</v>
       </c>
-      <c r="I37">
+      <c r="I31" s="4">
         <v>11.2</v>
       </c>
     </row>

</xml_diff>